<commit_message>
First Test using Test Vector in Excel Sheet. Red digits are missing.
</commit_message>
<xml_diff>
--- a/Sudoku.xlsx
+++ b/Sudoku.xlsx
@@ -8,20 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestVector" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,6 +35,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -249,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,13 +383,73 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -862,7 +925,7 @@
   <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -872,57 +935,85 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B2" s="23"/>
+      <c r="B2" s="49">
+        <v>7</v>
+      </c>
       <c r="C2" s="24">
         <v>8</v>
       </c>
-      <c r="D2" s="42"/>
+      <c r="D2" s="50">
+        <v>9</v>
+      </c>
       <c r="E2" s="31">
         <v>4</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="45">
+        <v>2</v>
+      </c>
       <c r="G2" s="39">
         <v>1</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="49">
+        <v>3</v>
+      </c>
       <c r="I2" s="24">
         <v>5</v>
       </c>
-      <c r="J2" s="42"/>
+      <c r="J2" s="50">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B3" s="29"/>
+      <c r="B3" s="51">
+        <v>4</v>
+      </c>
       <c r="C3" s="25">
         <v>5</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="52">
+        <v>6</v>
+      </c>
       <c r="E3" s="36">
         <v>3</v>
       </c>
       <c r="F3" s="40">
         <v>9</v>
       </c>
-      <c r="G3" s="32"/>
+      <c r="G3" s="46">
+        <v>8</v>
+      </c>
       <c r="H3" s="29">
         <v>1</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="55">
+        <v>7</v>
+      </c>
       <c r="J3" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B4" s="33"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="53">
+        <v>3</v>
+      </c>
+      <c r="C4" s="54">
+        <v>1</v>
+      </c>
       <c r="D4" s="30">
         <v>2</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="47">
+        <v>5</v>
+      </c>
       <c r="F4" s="38">
         <v>7</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="33"/>
+      <c r="G4" s="48">
+        <v>6</v>
+      </c>
+      <c r="H4" s="53">
+        <v>8</v>
+      </c>
       <c r="I4" s="26">
         <v>9</v>
       </c>
@@ -940,72 +1031,116 @@
       <c r="D5" s="39">
         <v>1</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="49">
+        <v>7</v>
+      </c>
+      <c r="F5" s="59">
+        <v>4</v>
+      </c>
       <c r="G5" s="34">
         <v>3</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="44"/>
+      <c r="H5" s="61">
+        <v>5</v>
+      </c>
+      <c r="I5" s="45">
+        <v>6</v>
+      </c>
+      <c r="J5" s="62">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B6" s="36"/>
-      <c r="C6" s="40"/>
+      <c r="B6" s="56">
+        <v>8</v>
+      </c>
+      <c r="C6" s="57">
+        <v>6</v>
+      </c>
       <c r="D6" s="32">
         <v>7</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="51">
+        <v>9</v>
+      </c>
       <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="60">
+        <v>5</v>
+      </c>
       <c r="H6" s="36">
         <v>2</v>
       </c>
       <c r="I6" s="40">
         <v>4</v>
       </c>
-      <c r="J6" s="45"/>
+      <c r="J6" s="63">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="2:10" ht="27.75" customHeight="1" thickBot="1">
       <c r="B7" s="41">
         <v>5</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="28"/>
+      <c r="C7" s="58">
+        <v>4</v>
+      </c>
+      <c r="D7" s="48">
+        <v>3</v>
+      </c>
       <c r="E7" s="33">
         <v>8</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="46">
+      <c r="F7" s="54">
+        <v>6</v>
+      </c>
+      <c r="G7" s="44">
         <v>2</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="37"/>
+      <c r="H7" s="47">
+        <v>7</v>
+      </c>
+      <c r="I7" s="58">
+        <v>1</v>
+      </c>
+      <c r="J7" s="64">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B8" s="23"/>
+      <c r="B8" s="49">
+        <v>6</v>
+      </c>
       <c r="C8" s="24">
         <v>7</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="65">
+        <v>8</v>
+      </c>
       <c r="E8" s="31">
         <v>1</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="45">
+        <v>3</v>
+      </c>
       <c r="G8" s="39">
         <v>4</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
+      <c r="H8" s="49">
+        <v>9</v>
+      </c>
+      <c r="I8" s="59">
+        <v>2</v>
+      </c>
       <c r="J8" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B9" s="29"/>
+      <c r="B9" s="51">
+        <v>1</v>
+      </c>
       <c r="C9" s="25">
         <v>3</v>
       </c>
@@ -1015,15 +1150,21 @@
       <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="40"/>
+      <c r="F9" s="57">
+        <v>5</v>
+      </c>
       <c r="G9" s="32">
         <v>9</v>
       </c>
       <c r="H9" s="29">
         <v>6</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="43"/>
+      <c r="I9" s="55">
+        <v>8</v>
+      </c>
+      <c r="J9" s="52">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="27.75" customHeight="1" thickBot="1">
       <c r="B10" s="33">
@@ -1032,14 +1173,24 @@
       <c r="C10" s="26">
         <v>2</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="41"/>
+      <c r="D10" s="66">
+        <v>5</v>
+      </c>
+      <c r="E10" s="47">
+        <v>6</v>
+      </c>
       <c r="F10" s="38">
         <v>8</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="26"/>
+      <c r="G10" s="48">
+        <v>7</v>
+      </c>
+      <c r="H10" s="53">
+        <v>4</v>
+      </c>
+      <c r="I10" s="54">
+        <v>3</v>
+      </c>
       <c r="J10" s="30">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Optimize execution speed to prevent permutation of all digits up till last two if they exist in corresponding row/column.
</commit_message>
<xml_diff>
--- a/Sudoku.xlsx
+++ b/Sudoku.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="TestVector" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestVector1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -17,7 +17,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,6 +42,20 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -252,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,6 +464,123 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -924,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1203,12 +1334,281 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C2:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="11" width="5.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:11" ht="24.75" customHeight="1">
+      <c r="C3" s="67">
+        <v>5</v>
+      </c>
+      <c r="D3" s="88">
+        <v>1</v>
+      </c>
+      <c r="E3" s="69">
+        <v>4</v>
+      </c>
+      <c r="F3" s="90">
+        <v>7</v>
+      </c>
+      <c r="G3" s="87">
+        <v>6</v>
+      </c>
+      <c r="H3" s="71">
+        <v>3</v>
+      </c>
+      <c r="I3" s="67">
+        <v>2</v>
+      </c>
+      <c r="J3" s="88">
+        <v>8</v>
+      </c>
+      <c r="K3" s="69">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" ht="24.75" customHeight="1">
+      <c r="C4" s="72">
+        <v>8</v>
+      </c>
+      <c r="D4" s="79">
+        <v>2</v>
+      </c>
+      <c r="E4" s="80">
+        <v>6</v>
+      </c>
+      <c r="F4" s="75">
+        <v>9</v>
+      </c>
+      <c r="G4" s="92">
+        <v>1</v>
+      </c>
+      <c r="H4" s="93">
+        <v>5</v>
+      </c>
+      <c r="I4" s="78">
+        <v>7</v>
+      </c>
+      <c r="J4" s="79">
+        <v>4</v>
+      </c>
+      <c r="K4" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="24.75" customHeight="1" thickBot="1">
+      <c r="C5" s="81">
+        <v>3</v>
+      </c>
+      <c r="D5" s="86">
+        <v>9</v>
+      </c>
+      <c r="E5" s="104">
+        <v>7</v>
+      </c>
+      <c r="F5" s="83">
+        <v>2</v>
+      </c>
+      <c r="G5" s="96">
+        <v>8</v>
+      </c>
+      <c r="H5" s="85">
+        <v>4</v>
+      </c>
+      <c r="I5" s="81">
+        <v>6</v>
+      </c>
+      <c r="J5" s="82">
+        <v>1</v>
+      </c>
+      <c r="K5" s="104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" ht="24.75" customHeight="1">
+      <c r="C6" s="90">
+        <v>2</v>
+      </c>
+      <c r="D6" s="87">
+        <v>8</v>
+      </c>
+      <c r="E6" s="71">
+        <v>3</v>
+      </c>
+      <c r="F6" s="67">
+        <v>1</v>
+      </c>
+      <c r="G6" s="88">
+        <v>4</v>
+      </c>
+      <c r="H6" s="89">
+        <v>6</v>
+      </c>
+      <c r="I6" s="90">
+        <v>9</v>
+      </c>
+      <c r="J6" s="70">
+        <v>5</v>
+      </c>
+      <c r="K6" s="102">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="24.75" customHeight="1">
+      <c r="C7" s="75">
+        <v>4</v>
+      </c>
+      <c r="D7" s="76">
+        <v>6</v>
+      </c>
+      <c r="E7" s="77">
+        <v>9</v>
+      </c>
+      <c r="F7" s="72">
+        <v>5</v>
+      </c>
+      <c r="G7" s="73">
+        <v>7</v>
+      </c>
+      <c r="H7" s="94">
+        <v>2</v>
+      </c>
+      <c r="I7" s="91">
+        <v>1</v>
+      </c>
+      <c r="J7" s="76">
+        <v>3</v>
+      </c>
+      <c r="K7" s="103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" ht="24.75" customHeight="1" thickBot="1">
+      <c r="C8" s="95">
+        <v>1</v>
+      </c>
+      <c r="D8" s="96">
+        <v>7</v>
+      </c>
+      <c r="E8" s="85">
+        <v>5</v>
+      </c>
+      <c r="F8" s="97">
+        <v>3</v>
+      </c>
+      <c r="G8" s="82">
+        <v>9</v>
+      </c>
+      <c r="H8" s="101">
+        <v>8</v>
+      </c>
+      <c r="I8" s="95">
+        <v>4</v>
+      </c>
+      <c r="J8" s="84">
+        <v>2</v>
+      </c>
+      <c r="K8" s="98">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" ht="24.75" customHeight="1">
+      <c r="C9" s="67">
+        <v>7</v>
+      </c>
+      <c r="D9" s="88">
+        <v>3</v>
+      </c>
+      <c r="E9" s="99">
+        <v>2</v>
+      </c>
+      <c r="F9" s="90">
+        <v>6</v>
+      </c>
+      <c r="G9" s="70">
+        <v>5</v>
+      </c>
+      <c r="H9" s="105">
+        <v>1</v>
+      </c>
+      <c r="I9" s="67">
+        <v>8</v>
+      </c>
+      <c r="J9" s="68">
+        <v>9</v>
+      </c>
+      <c r="K9" s="69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" ht="24.75" customHeight="1">
+      <c r="C10" s="72">
+        <v>9</v>
+      </c>
+      <c r="D10" s="79">
+        <v>4</v>
+      </c>
+      <c r="E10" s="100">
+        <v>1</v>
+      </c>
+      <c r="F10" s="75">
+        <v>8</v>
+      </c>
+      <c r="G10" s="92">
+        <v>3</v>
+      </c>
+      <c r="H10" s="93">
+        <v>7</v>
+      </c>
+      <c r="I10" s="78">
+        <v>5</v>
+      </c>
+      <c r="J10" s="79">
+        <v>6</v>
+      </c>
+      <c r="K10" s="74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="24.75" customHeight="1" thickBot="1">
+      <c r="C11" s="81">
+        <v>6</v>
+      </c>
+      <c r="D11" s="82">
+        <v>5</v>
+      </c>
+      <c r="E11" s="101">
+        <v>8</v>
+      </c>
+      <c r="F11" s="95">
+        <v>4</v>
+      </c>
+      <c r="G11" s="84">
+        <v>2</v>
+      </c>
+      <c r="H11" s="85">
+        <v>9</v>
+      </c>
+      <c r="I11" s="81">
+        <v>3</v>
+      </c>
+      <c r="J11" s="82">
+        <v>7</v>
+      </c>
+      <c r="K11" s="104">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>